<commit_message>
add book exmaple code
</commit_message>
<xml_diff>
--- a/FEDAI/Errata/Errata of FEIDA datalist.xlsx
+++ b/FEDAI/Errata/Errata of FEIDA datalist.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yy2633/MA/2019Spring/RAship/FEDAI/Errata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6429262F-BD9D-014B-957B-687F01766DAE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0AAC16-035B-A242-8E26-7575A567708C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="500" windowWidth="25740" windowHeight="17040" xr2:uid="{5E06B9E7-531E-1848-A504-08FDF6D3C7A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Errata" sheetId="2" r:id="rId1"/>
+    <sheet name="label for csv" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -279,6 +280,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -287,18 +300,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -620,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AABB73-E0F1-FF4D-98A2-4D18D33E7DF1}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A18" sqref="A18:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -636,22 +637,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="38" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
@@ -669,10 +670,10 @@
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -692,7 +693,7 @@
       <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -706,16 +707,16 @@
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -752,7 +753,7 @@
       <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -769,72 +770,18 @@
       <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1"/>
     <row r="16" spans="1:5" s="4" customFormat="1"/>
-    <row r="17" spans="2:5" s="4" customFormat="1"/>
-    <row r="18" spans="2:5" s="4" customFormat="1"/>
-    <row r="19" spans="2:5" ht="35">
-      <c r="B19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
+    <row r="17" s="4" customFormat="1"/>
+    <row r="18" s="4" customFormat="1"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -842,4 +789,87 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6CC20D-01ED-0F4F-ABC9-1B1A74CD7F7B}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="52.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" customWidth="1"/>
+    <col min="3" max="3" width="68" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="35">
+      <c r="A2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
PDF demo R to Stata
</commit_message>
<xml_diff>
--- a/FEDAI/Errata/Errata of FEIDA datalist.xlsx
+++ b/FEDAI/Errata/Errata of FEIDA datalist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yy2633/MA/2019Spring/RAship/FEDAI/Errata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yy2633/MA/RAship/FEDAI/Errata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0AAC16-035B-A242-8E26-7575A567708C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90682440-B306-D94F-8C41-77E6188E1862}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="500" windowWidth="25740" windowHeight="17040" xr2:uid="{5E06B9E7-531E-1848-A504-08FDF6D3C7A1}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:E24"/>
+      <selection activeCell="E10" sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>